<commit_message>
changed csv output to excel
</commit_message>
<xml_diff>
--- a/RPAfinalProject/outputLaptopsTable.xlsx
+++ b/RPAfinalProject/outputLaptopsTable.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <x:si>
+    <x:t>Titlu laptop</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Link laptop</x:t>
+  </x:si>
   <x:si>
     <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ACH6, FHD IPS, Procesor AMD Ryzen™ 5 5600H (16M Cache, up to 4.2 GHz), 16GB DDR4, 512GB SSD, GeForce RTX 3050 4GB, No OS, Shadow Black</x:t>
   </x:si>
@@ -430,266 +436,274 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D32"/>
+  <x:dimension ref="A1:B33"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
-      <x:c r="C1" s="0" t="s">
+    <x:row r="1" spans="1:2">
+      <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="D1" s="0" t="s">
+      <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:4">
-      <x:c r="C2" s="0" t="s">
+    <x:row r="2" spans="1:2">
+      <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:4">
-      <x:c r="C3" s="0" t="s">
+    <x:row r="3" spans="1:2">
+      <x:c r="A3" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s">
+      <x:c r="B3" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4">
-      <x:c r="C4" s="0" t="s">
+    <x:row r="4" spans="1:2">
+      <x:c r="A4" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D4" s="0" t="s">
+      <x:c r="B4" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:4">
-      <x:c r="C5" s="0" t="s">
+    <x:row r="5" spans="1:2">
+      <x:c r="A5" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="D5" s="0" t="s">
+      <x:c r="B5" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:4">
-      <x:c r="C6" s="0" t="s">
+    <x:row r="6" spans="1:2">
+      <x:c r="A6" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="D6" s="0" t="s">
+      <x:c r="B6" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:4">
-      <x:c r="C7" s="0" t="s">
+    <x:row r="7" spans="1:2">
+      <x:c r="A7" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D7" s="0" t="s">
+      <x:c r="B7" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:4">
-      <x:c r="C8" s="0" t="s">
+    <x:row r="8" spans="1:2">
+      <x:c r="A8" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="D8" s="0" t="s">
+      <x:c r="B8" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:4">
-      <x:c r="C9" s="0" t="s">
+    <x:row r="9" spans="1:2">
+      <x:c r="A9" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="D9" s="0" t="s">
+      <x:c r="B9" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:4">
-      <x:c r="C10" s="0" t="s">
+    <x:row r="10" spans="1:2">
+      <x:c r="A10" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="D10" s="0" t="s">
+      <x:c r="B10" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:4">
-      <x:c r="C11" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="D11" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:4">
-      <x:c r="C12" s="0" t="s">
+    <x:row r="11" spans="1:2">
+      <x:c r="A11" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:2">
+      <x:c r="A12" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D12" s="0" t="s">
+      <x:c r="B12" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:4">
-      <x:c r="C13" s="0" t="s">
+    <x:row r="13" spans="1:2">
+      <x:c r="A13" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="D13" s="0" t="s">
+      <x:c r="B13" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:4">
-      <x:c r="C14" s="0" t="s">
+    <x:row r="14" spans="1:2">
+      <x:c r="A14" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D14" s="0" t="s">
+      <x:c r="B14" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:4">
-      <x:c r="C15" s="0" t="s">
+    <x:row r="15" spans="1:2">
+      <x:c r="A15" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="D15" s="0" t="s">
+      <x:c r="B15" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:4">
-      <x:c r="C16" s="0" t="s">
+    <x:row r="16" spans="1:2">
+      <x:c r="A16" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="D16" s="0" t="s">
+      <x:c r="B16" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:4">
-      <x:c r="C17" s="0" t="s">
+    <x:row r="17" spans="1:2">
+      <x:c r="A17" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D17" s="0" t="s">
+      <x:c r="B17" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:4">
-      <x:c r="C18" s="0" t="s">
+    <x:row r="18" spans="1:2">
+      <x:c r="A18" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="D18" s="0" t="s">
+      <x:c r="B18" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:4">
-      <x:c r="C19" s="0" t="s">
+    <x:row r="19" spans="1:2">
+      <x:c r="A19" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="D19" s="0" t="s">
+      <x:c r="B19" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:4">
-      <x:c r="C20" s="0" t="s">
+    <x:row r="20" spans="1:2">
+      <x:c r="A20" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="D20" s="0" t="s">
+      <x:c r="B20" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:4">
-      <x:c r="C21" s="0" t="s">
+    <x:row r="21" spans="1:2">
+      <x:c r="A21" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="D21" s="0" t="s">
+      <x:c r="B21" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
-    <x:row r="22" spans="1:4">
-      <x:c r="C22" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="D22" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:4">
-      <x:c r="C23" s="0" t="s">
+    <x:row r="22" spans="1:2">
+      <x:c r="A22" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:2">
+      <x:c r="A23" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D23" s="0" t="s">
+      <x:c r="B23" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="24" spans="1:4">
-      <x:c r="C24" s="0" t="s">
+    <x:row r="24" spans="1:2">
+      <x:c r="A24" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="D24" s="0" t="s">
+      <x:c r="B24" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="25" spans="1:4">
-      <x:c r="C25" s="0" t="s">
+    <x:row r="25" spans="1:2">
+      <x:c r="A25" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="D25" s="0" t="s">
+      <x:c r="B25" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="26" spans="1:4">
-      <x:c r="C26" s="0" t="s">
+    <x:row r="26" spans="1:2">
+      <x:c r="A26" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="D26" s="0" t="s">
+      <x:c r="B26" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="27" spans="1:4">
-      <x:c r="C27" s="0" t="s">
+    <x:row r="27" spans="1:2">
+      <x:c r="A27" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="D27" s="0" t="s">
+      <x:c r="B27" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="28" spans="1:4">
-      <x:c r="C28" s="0" t="s">
+    <x:row r="28" spans="1:2">
+      <x:c r="A28" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="D28" s="0" t="s">
+      <x:c r="B28" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="29" spans="1:4">
-      <x:c r="C29" s="0" t="s">
+    <x:row r="29" spans="1:2">
+      <x:c r="A29" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="D29" s="0" t="s">
+      <x:c r="B29" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
     </x:row>
-    <x:row r="30" spans="1:4">
-      <x:c r="C30" s="0" t="s">
+    <x:row r="30" spans="1:2">
+      <x:c r="A30" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="D30" s="0" t="s">
+      <x:c r="B30" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="31" spans="1:4">
-      <x:c r="C31" s="0" t="s">
+    <x:row r="31" spans="1:2">
+      <x:c r="A31" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="D31" s="0" t="s">
+      <x:c r="B31" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
     </x:row>
-    <x:row r="32" spans="1:4">
-      <x:c r="C32" s="0" t="s">
+    <x:row r="32" spans="1:2">
+      <x:c r="A32" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="D32" s="0" t="s">
+      <x:c r="B32" s="0" t="s">
         <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:2">
+      <x:c r="A33" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>23</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
without csv for debug
</commit_message>
<xml_diff>
--- a/RPAfinalProject/outputLaptopsTable.xlsx
+++ b/RPAfinalProject/outputLaptopsTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <x:si>
     <x:t>Titlu laptop</x:t>
   </x:si>
@@ -22,70 +22,16 @@
     <x:t>Link laptop</x:t>
   </x:si>
   <x:si>
-    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ACH6, FHD IPS, Procesor AMD Ryzen™ 5 5600H (16M Cache, up to 4.2 GHz), 16GB DDR4, 512GB SSD, GeForce RTX 3050 4GB, No OS, Shadow Black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15ach6-fhd-ips-procesor-amd-ryzen-5-5600h-16m-cache-up-to-42-ghz-16gb-ddr4-512gb-ssd-geforce-rtx-3050-4gb-no-os-shadow-black/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ACH6, FHD IPS 120Hz, Procesor AMD Ryzen™ 5 5600H (16M Cache, up to 4.2 GHz), 16GB DDR4, 512GB SSD, GeForce RTX 3050 Ti 4GB, No OS, Shadow Black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15ach6-fhd-ips-120hz-procesor-amd-ryzen-5-5600h-16m-cache-up-to-42-ghz-16gb-ddr4-512gb-ssd-geforce-rtx-3050-ti-4gb-no-os-shadow-black/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ACH6, FHD IPS, Procesor AMD Ryzen™ 7 5800H (16M Cache, up to 4.4 GHz), 16GB DDR4, 512GB SSD, GeForce RTX 3050 4GB, No OS, Shadow Black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15ach6-fhd-ips-procesor-amd-ryzen-7-5800h-16m-cache-up-to-44-ghz-16gb-ddr4-512gb-ssd-geforce-rtx-3050-4gb-no-os-shadow-black/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ACH6, FHD IPS 120Hz, Procesor AMD Ryzen™ 7 5800H (16M Cache, up to 4.4 GHz), 16GB DDR4, 512GB SSD, GeForce RTX 3050 Ti 4GB, No OS, Shadow Black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15ach6-fhd-ips-120hz-procesor-amd-ryzen-7-5800h-16m-cache-up-to-44-ghz-16gb-ddr4-512gb-ssd-geforce-rtx-3050-ti-4gb-no-os-shadow-black-1/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ARH7, FHD IPS 120Hz, Procesor AMD Ryzen™ 5 6600H (16M Cache, up to 4.5 GHz), 16GB DDR5, 512GB SSD, GeForce RTX 3050 Ti 4GB, No OS, Onyx Grey</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15arh7-fhd-ips-120hz-procesor-amd-ryzen-5-6600h-16m-cache-up-to-45-ghz-16gb-ddr5-512gb-ssd-geforce-rtx-3050-ti-4gb-no-os-onyx-grey/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ARH7, FHD IPS 120Hz, Procesor AMD Ryzen™ 7 6800H (16M Cache, up to 4.7 GHz), 16GB DDR5, 512GB SSD, GeForce RTX 3050 Ti 4GB, No OS, Glacier White</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15arh7-fhd-ips-120hz-procesor-amd-ryzen-7-6800h-16m-cache-up-to-47-ghz-16gb-ddr5-512gb-ssd-geforce-rtx-3050-ti-4gb-no-os-glacier-white/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ACH6, FHD IPS 120Hz, Procesor AMD Ryzen™ 7 5800H (16M Cache, up to 4.4 GHz), 16GB DDR4, 512GB SSD, GeForce RTX 3050 4GB, No OS, Shadow Black, 4-Zone RGB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15ach6-fhd-ips-120hz-procesor-amd-ryzen-7-5800h-16m-cache-up-to-44-ghz-16gb-ddr4-512gb-ssd-geforce-rtx-3050-4gb-no-os-shadow-black-4-zone-rgb/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Laptop Lenovo Gaming 15.6'' Legion 5 15ARH05, FHD IPS 120Hz, Procesor AMD Ryzen™ 5 4600H (8M Cache, up to 4.0 GHz), 16GB DDR4, 512GB SSD, GeForce GTX 1650 4GB, No OS, Phantom Black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-legion-5-15arh05-fhd-ips-120hz-procesor-amd-ryzen-5-4600h-8m-cache-up-to-40-ghz-16gb-ddr4-512gb-ssd-geforce-gtx-1650-4gb-no-os-phantom-black/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ACH6, FHD IPS 165Hz, Procesor AMD Ryzen™ 5 5600H (16M Cache, up to 4.2 GHz), 16GB DDR4, 512GB SSD, GeForce RTX 3050 Ti 4GB, No OS, Shadow Black, 4-Zone RGB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15ach6-fhd-ips-165hz-procesor-amd-ryzen-5-5600h-16m-cache-up-to-42-ghz-16gb-ddr4-512gb-ssd-geforce-rtx-3050-ti-4gb-no-os-shadow-black-4-zone-rgb/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Laptop Lenovo Gaming 15.6'' Legion 5 15ARH05, FHD IPS 144Hz, Procesor AMD Ryzen™ 5 4600H (8M Cache, up to 4.0 GHz), 16GB DDR4, 512GB SSD, GeForce GTX 1650 4GB, No OS, Phantom Black, 4-Zone RGB</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-legion-5-15arh05-fhd-ips-144hz-procesor-amd-ryzen-5-4600h-8m-cache-up-to-40-ghz-16gb-ddr4-512gb-ssd-geforce-gtx-1650-4gb-no-os-phantom-black-4-zone-rgb/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Laptop gaming LENOVO IdeaPad Gaming 3 15IAH7, Intel Core i5-12450H pana la 4.4GHz, 15.6" Full HD, 16GB, SSD 512GB, NVIDIA GeForce RTX 3050 Ti 4GB, Free DOS, Onyx Grey</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://altex.ro/laptop-gaming-lenovo-ideapad-gaming-3-15iah7-intel-core-i5-12450h-pana-la-4-4ghz-15-6-full-hd-16gb-ssd-512gb-nvidia-geforce-rtx-3050-ti-4gb-free-dos-onyx-grey/cpd/LAP82S900KKRM/</x:t>
+    <x:t>Laptop ASUS Vivobook Pro 14X OLED M7400QE-KM008W, 14" 2.8K, AMD Ryzen 7 5800H pana la 4.4GHz, 16GB, SSD 512GB, NVIDIA GeForce RTX 3050Ti 4GB, Windows 11 Home, negru</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://altex.ro/laptop-asus-vivobook-pro-14x-oled-m7400qe-km008w-14-2-8k-amd-ryzen-7-5800h-pana-la-4-4ghz-16gb-ssd-512gb-nvidia-geforce-rtx-3050ti-4gb-windows-11-home-negru/cpd/LAPM7400QKM007W/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop ASUS Zenbook Pro 15 UX535LI cu procesor Intel® Core™ i5-10300H, 15.6", Full HD, 8GB, 1TB HDD + 512GB SSD, NVIDIA® GeForce® GTX 1650 Ti 4GB, Windows 10 Home, Pine Grey</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.emag.ro/laptop-asus-zenbook-pro-15-ux535li-cu-procesor-intelr-coretm-i5-10300h-15-6-full-hd-8gb-1tb-hdd-512gb-ssd-nvidiar-geforcer-gtx-1650-ti-4gb-windows-10-home-pine-grey-ux535li-bn025t/pd/DQLCLKMBM/?</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -436,7 +382,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B33"/>
+  <x:dimension ref="A1:B3"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -464,246 +410,6 @@
       </x:c>
       <x:c r="B3" s="0" t="s">
         <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:2">
-      <x:c r="A4" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:2">
-      <x:c r="A5" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:2">
-      <x:c r="A6" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:2">
-      <x:c r="A7" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:2">
-      <x:c r="A8" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:2">
-      <x:c r="A9" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:2">
-      <x:c r="A10" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:2">
-      <x:c r="A11" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:2">
-      <x:c r="A12" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B12" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:2">
-      <x:c r="A13" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B13" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:2">
-      <x:c r="A14" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B14" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:2">
-      <x:c r="A15" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B15" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:2">
-      <x:c r="A16" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:2">
-      <x:c r="A17" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B17" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:2">
-      <x:c r="A18" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B18" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:2">
-      <x:c r="A19" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B19" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:2">
-      <x:c r="A20" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B20" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:2">
-      <x:c r="A21" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B21" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:2">
-      <x:c r="A22" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="B22" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:2">
-      <x:c r="A23" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B23" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:2">
-      <x:c r="A24" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B24" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:2">
-      <x:c r="A25" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B25" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:2">
-      <x:c r="A26" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B26" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:2">
-      <x:c r="A27" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B27" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:2">
-      <x:c r="A28" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B28" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:2">
-      <x:c r="A29" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B29" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="1:2">
-      <x:c r="A30" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B30" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:2">
-      <x:c r="A31" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B31" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:2">
-      <x:c r="A32" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B32" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:2">
-      <x:c r="A33" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="B33" s="0" t="s">
-        <x:v>23</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Added invalid input mail
</commit_message>
<xml_diff>
--- a/RPAfinalProject/outputLaptopsTable.xlsx
+++ b/RPAfinalProject/outputLaptopsTable.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <x:si>
     <x:t>Titlu laptop</x:t>
   </x:si>
@@ -22,16 +22,94 @@
     <x:t>Link laptop</x:t>
   </x:si>
   <x:si>
-    <x:t>Laptop ASUS Vivobook Pro 14X OLED M7400QE-KM008W, 14" 2.8K, AMD Ryzen 7 5800H pana la 4.4GHz, 16GB, SSD 512GB, NVIDIA GeForce RTX 3050Ti 4GB, Windows 11 Home, negru</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://altex.ro/laptop-asus-vivobook-pro-14x-oled-m7400qe-km008w-14-2-8k-amd-ryzen-7-5800h-pana-la-4-4ghz-16gb-ssd-512gb-nvidia-geforce-rtx-3050ti-4gb-windows-11-home-negru/cpd/LAPM7400QKM007W/</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Laptop ASUS Zenbook Pro 15 UX535LI cu procesor Intel® Core™ i5-10300H, 15.6", Full HD, 8GB, 1TB HDD + 512GB SSD, NVIDIA® GeForce® GTX 1650 Ti 4GB, Windows 10 Home, Pine Grey</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.emag.ro/laptop-asus-zenbook-pro-15-ux535li-cu-procesor-intelr-coretm-i5-10300h-15-6-full-hd-8gb-1tb-hdd-512gb-ssd-nvidiar-geforcer-gtx-1650-ti-4gb-windows-10-home-pine-grey-ux535li-bn025t/pd/DQLCLKMBM/?</x:t>
+    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ACH6, FHD IPS, Procesor AMD Ryzen™ 5 5600H (16M Cache, up to 4.2 GHz), 16GB DDR4, 512GB SSD, GeForce RTX 3050 4GB, No OS, Shadow Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15ach6-fhd-ips-procesor-amd-ryzen-5-5600h-16m-cache-up-to-42-ghz-16gb-ddr4-512gb-ssd-geforce-rtx-3050-4gb-no-os-shadow-black/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ACH6, FHD IPS 120Hz, Procesor AMD Ryzen™ 5 5600H (16M Cache, up to 4.2 GHz), 16GB DDR4, 512GB SSD, GeForce RTX 3050 Ti 4GB, No OS, Shadow Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15ach6-fhd-ips-120hz-procesor-amd-ryzen-5-5600h-16m-cache-up-to-42-ghz-16gb-ddr4-512gb-ssd-geforce-rtx-3050-ti-4gb-no-os-shadow-black/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ACH6, FHD IPS, Procesor AMD Ryzen™ 7 5800H (16M Cache, up to 4.4 GHz), 16GB DDR4, 512GB SSD, GeForce RTX 3050 4GB, No OS, Shadow Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15ach6-fhd-ips-procesor-amd-ryzen-7-5800h-16m-cache-up-to-44-ghz-16gb-ddr4-512gb-ssd-geforce-rtx-3050-4gb-no-os-shadow-black/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ACH6, FHD IPS 120Hz, Procesor AMD Ryzen™ 7 5800H (16M Cache, up to 4.4 GHz), 16GB DDR4, 512GB SSD, GeForce RTX 3050 Ti 4GB, No OS, Shadow Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15ach6-fhd-ips-120hz-procesor-amd-ryzen-7-5800h-16m-cache-up-to-44-ghz-16gb-ddr4-512gb-ssd-geforce-rtx-3050-ti-4gb-no-os-shadow-black-1/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ARH7, FHD IPS 120Hz, Procesor AMD Ryzen™ 5 6600H (16M Cache, up to 4.5 GHz), 16GB DDR5, 512GB SSD, GeForce RTX 3050 Ti 4GB, No OS, Onyx Grey</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15arh7-fhd-ips-120hz-procesor-amd-ryzen-5-6600h-16m-cache-up-to-45-ghz-16gb-ddr5-512gb-ssd-geforce-rtx-3050-ti-4gb-no-os-onyx-grey/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ARH7, FHD IPS 120Hz, Procesor AMD Ryzen™ 7 6800H (16M Cache, up to 4.7 GHz), 16GB DDR5, 512GB SSD, GeForce RTX 3050 Ti 4GB, No OS, Glacier White</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15arh7-fhd-ips-120hz-procesor-amd-ryzen-7-6800h-16m-cache-up-to-47-ghz-16gb-ddr5-512gb-ssd-geforce-rtx-3050-ti-4gb-no-os-glacier-white/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ACH6, FHD IPS 120Hz, Procesor AMD Ryzen™ 7 5800H (16M Cache, up to 4.4 GHz), 16GB DDR4, 512GB SSD, GeForce RTX 3050 4GB, No OS, Shadow Black, 4-Zone RGB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15ach6-fhd-ips-120hz-procesor-amd-ryzen-7-5800h-16m-cache-up-to-44-ghz-16gb-ddr4-512gb-ssd-geforce-rtx-3050-4gb-no-os-shadow-black-4-zone-rgb/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop Lenovo Gaming 15.6'' Legion 5 15ARH05, FHD IPS 120Hz, Procesor AMD Ryzen™ 5 4600H (8M Cache, up to 4.0 GHz), 16GB DDR4, 512GB SSD, GeForce GTX 1650 4GB, No OS, Phantom Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-legion-5-15arh05-fhd-ips-120hz-procesor-amd-ryzen-5-4600h-8m-cache-up-to-40-ghz-16gb-ddr4-512gb-ssd-geforce-gtx-1650-4gb-no-os-phantom-black/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop Lenovo Gaming 15.6'' IdeaPad 3 15ACH6, FHD IPS 165Hz, Procesor AMD Ryzen™ 5 5600H (16M Cache, up to 4.2 GHz), 16GB DDR4, 512GB SSD, GeForce RTX 3050 Ti 4GB, No OS, Shadow Black, 4-Zone RGB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-ideapad-3-15ach6-fhd-ips-165hz-procesor-amd-ryzen-5-5600h-16m-cache-up-to-42-ghz-16gb-ddr4-512gb-ssd-geforce-rtx-3050-ti-4gb-no-os-shadow-black-4-zone-rgb/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop Lenovo Gaming 15.6'' Legion 5 15ARH05, FHD IPS 144Hz, Procesor AMD Ryzen™ 5 4600H (8M Cache, up to 4.0 GHz), 16GB DDR4, 512GB SSD, GeForce GTX 1650 4GB, No OS, Phantom Black, 4-Zone RGB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.pcgarage.ro/notebook-laptop/lenovo/gaming-156-legion-5-15arh05-fhd-ips-144hz-procesor-amd-ryzen-5-4600h-8m-cache-up-to-40-ghz-16gb-ddr4-512gb-ssd-geforce-gtx-1650-4gb-no-os-phantom-black-4-zone-rgb/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop gaming LENOVO IdeaPad Gaming 3 15IAH7, Intel Core i5-12450H pana la 4.4GHz, 15.6" Full HD, 16GB, SSD 512GB, NVIDIA GeForce RTX 3050 Ti 4GB, Free DOS, Onyx Grey</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://altex.ro/laptop-gaming-lenovo-ideapad-gaming-3-15iah7-intel-core-i5-12450h-pana-la-4-4ghz-15-6-full-hd-16gb-ssd-512gb-nvidia-geforce-rtx-3050-ti-4gb-free-dos-onyx-grey/cpd/LAP82S900KKRM/</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop Gaming Lenovo IdeaPad 3 15ACH6 cu procesor AMD Ryzen™ 7 5800H pana la 4.40 GHz, 15.6", Full HD, IPS, 16GB, 512GB SSD, NVIDIA GeForce RTX 3050 4GB, No OS, Shadow Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.emag.ro/laptop-gaming-lenovo-ideapad-3-15ach6-cu-procesor-amd-ryzentm-7-5800h-pana-la-4-40-ghz-15-6-full-hd-ips-16gb-512gb-ssd-nvidia-geforce-rtx-3050-4gb-no-os-shadow-black-82k201sfrm/pd/DHP2W4MBM/?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop Gaming Lenovo IdeaPad 3 15ACH6 cu procesor AMD Ryzen™ 7 5800H pana la 4.40 GHz, 15.6'', Full HD, IPS, 120Hz, 16GB, 512GB SSD, NVIDIA GeForce RTX 3050 Ti 4GB, No OS, Shadow Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.emag.ro/laptop-gaming-lenovo-ideapad-3-15ach6-cu-procesor-amd-ryzentm-7-5800h-pana-la-4-40-ghz-15-6-full-hd-ips-120hz-16gb-512gb-ssd-nvidia-geforce-rtx-3050-ti-4gb-no-os-shadow-black-82k201usrm/pd/DN6Y8LMBM/?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop Gaming Lenovo IdeaPad 3 15ACH6 cu procesor AMD Ryzen™ 5 5600H pana la 4.20 GHz, 15.6", Full HD, IPS, 16GB, 512GB SSD, NVIDIA GeForce RTX 3050 4GB, No OS, Shadow Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.emag.ro/laptop-gaming-lenovo-ideapad-3-15ach6-cu-procesor-amd-ryzentm-5-5600h-pana-la-4-20-ghz-15-6-full-hd-ips-16gb-512gb-ssd-nvidia-geforce-rtx-3050-4gb-no-os-shadow-black-82k201sgrm/pd/DF9XMCMBM/?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Laptop Gaming LENOVO IdeaPad Gaming 3 15ACH6, AMD Ryzen 5 5600H pana la 4.2GHz, 15.6" Full HD, 16GB, SSD 512GB, NVIDIA GeForce GTX 1650, Free DOS, negru</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.emag.ro/laptop-gaming-lenovo-ideapad-gaming-3-15ach6-amd-ryzen-5-5600h-pana-la-4-2ghz-15-6-full-hd-16gb-ssd-512gb-nvidia-geforce-gtx-1650-free-dos-negru-82k2008krm/pd/DCH53JMBM/?</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -412,6 +490,110 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
+    <x:row r="4" spans="1:2">
+      <x:c r="A4" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:2">
+      <x:c r="A5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:2">
+      <x:c r="A6" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:2">
+      <x:c r="A7" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:2">
+      <x:c r="A8" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:2">
+      <x:c r="A9" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:2">
+      <x:c r="A10" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:2">
+      <x:c r="A11" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:2">
+      <x:c r="A12" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:2">
+      <x:c r="A13" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:2">
+      <x:c r="A14" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:2">
+      <x:c r="A15" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:2">
+      <x:c r="A16" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>